<commit_message>
type =PRODUCT(d5:e5) to get the gross salary in column f5
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4326B8-B0C2-4379-A151-AFE0B1D453A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59091D-A27A-4833-AC4D-D4E68CBD2304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +625,7 @@
         <v>2500</v>
       </c>
       <c r="F5" s="2">
+        <f>PRODUCT(D5:E5)</f>
         <v>100000</v>
       </c>
       <c r="G5" s="1">

</xml_diff>

<commit_message>
drag from cell f5 to cell f14 to apply the same function to those cells
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59091D-A27A-4833-AC4D-D4E68CBD2304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7956E133-DA77-4AE5-891E-C4A63EC65058}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +648,10 @@
       <c r="E6">
         <v>5000</v>
       </c>
+      <c r="F6" s="2">
+        <f t="shared" ref="F6:F14" si="0">PRODUCT(D6:E6)</f>
+        <v>360000</v>
+      </c>
       <c r="G6" s="1">
         <v>0.2</v>
       </c>
@@ -668,6 +672,10 @@
       <c r="E7">
         <v>5000</v>
       </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>315000</v>
+      </c>
       <c r="G7" s="1">
         <v>0.15</v>
       </c>
@@ -688,6 +696,10 @@
       <c r="E8">
         <v>5000</v>
       </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>260000</v>
+      </c>
       <c r="G8" s="1">
         <v>0.32</v>
       </c>
@@ -708,6 +720,10 @@
       <c r="E9">
         <v>6500</v>
       </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>435500</v>
+      </c>
       <c r="G9" s="1">
         <v>0.15</v>
       </c>
@@ -728,6 +744,10 @@
       <c r="E10">
         <v>4500</v>
       </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
@@ -748,6 +768,10 @@
       <c r="E11">
         <v>1200</v>
       </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>91200</v>
+      </c>
       <c r="G11" s="1">
         <v>0.25</v>
       </c>
@@ -768,6 +792,10 @@
       <c r="E12">
         <v>3200</v>
       </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>284800</v>
+      </c>
       <c r="G12" s="1">
         <v>0.4</v>
       </c>
@@ -788,6 +816,10 @@
       <c r="E13">
         <v>4000</v>
       </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>344000</v>
+      </c>
       <c r="G13" s="1">
         <v>0.15</v>
       </c>
@@ -807,6 +839,10 @@
       </c>
       <c r="E14">
         <v>2600</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>83200</v>
       </c>
       <c r="G14" s="1">
         <v>0.55000000000000004</v>

</xml_diff>

<commit_message>
type =(f5*g5) in cell h5 to get the 15% of 100000
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7956E133-DA77-4AE5-891E-C4A63EC65058}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C36EBD-8A0C-4A45-8A9D-20C9BC20553F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +631,10 @@
       <c r="G5" s="1">
         <v>0.15</v>
       </c>
+      <c r="H5">
+        <f>(F5*G5)</f>
+        <v>15000</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
drag down from cell h5 to cell h14 to apply the same function to all cells
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C36EBD-8A0C-4A45-8A9D-20C9BC20553F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3A6189-55BB-4639-8BC3-8A277E74D9AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,6 +659,10 @@
       <c r="G6" s="1">
         <v>0.2</v>
       </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H14" si="1">(F6*G6)</f>
+        <v>72000</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -683,6 +687,10 @@
       <c r="G7" s="1">
         <v>0.15</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>47250</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -707,6 +715,10 @@
       <c r="G8" s="1">
         <v>0.32</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>83200</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -731,6 +743,10 @@
       <c r="G9" s="1">
         <v>0.15</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>65325</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -755,6 +771,10 @@
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>54000</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -779,6 +799,10 @@
       <c r="G11" s="1">
         <v>0.25</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>22800</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -803,6 +827,10 @@
       <c r="G12" s="1">
         <v>0.4</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>113920</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -827,6 +855,10 @@
       <c r="G13" s="1">
         <v>0.15</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>51600</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -850,6 +882,10 @@
       </c>
       <c r="G14" s="1">
         <v>0.55000000000000004</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>45760.000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
type f5-h5 in cell i5 to get the net pay
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3A6189-55BB-4639-8BC3-8A277E74D9AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0730780-590F-4AE4-BD59-3A4DF35D5F73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,6 +635,10 @@
         <f>(F5*G5)</f>
         <v>15000</v>
       </c>
+      <c r="I5" s="2">
+        <f>F5-H5</f>
+        <v>85000</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
drag down from cell i5 to i14 to apply the same function to all those cells through to i14
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0730780-590F-4AE4-BD59-3A4DF35D5F73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114F853A-0341-4117-8357-EE5C26FDC97A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +667,10 @@
         <f t="shared" ref="H6:H14" si="1">(F6*G6)</f>
         <v>72000</v>
       </c>
+      <c r="I6" s="2">
+        <f t="shared" ref="I6:I14" si="2">F6-H6</f>
+        <v>288000</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -695,6 +699,10 @@
         <f t="shared" si="1"/>
         <v>47250</v>
       </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>267750</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -723,6 +731,10 @@
         <f t="shared" si="1"/>
         <v>83200</v>
       </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>176800</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -751,6 +763,10 @@
         <f t="shared" si="1"/>
         <v>65325</v>
       </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>370175</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -779,6 +795,10 @@
         <f t="shared" si="1"/>
         <v>54000</v>
       </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>306000</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -807,6 +827,10 @@
         <f t="shared" si="1"/>
         <v>22800</v>
       </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>68400</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -835,6 +859,10 @@
         <f t="shared" si="1"/>
         <v>113920</v>
       </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>170880</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -863,6 +891,10 @@
         <f t="shared" si="1"/>
         <v>51600</v>
       </c>
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>292400</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -890,6 +922,10 @@
       <c r="H14">
         <f t="shared" si="1"/>
         <v>45760.000000000007</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="2"/>
+        <v>37439.999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added bar chart to show how many hours each person is present for
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114F853A-0341-4117-8357-EE5C26FDC97A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B11698-44E9-4D08-B538-6A30F500C437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -169,6 +169,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +204,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,6 +220,1986 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hrs Present</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$5:$C$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Coding</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Food &amp; Beverage</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Coding</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Coding</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Early Childhood</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Cyber Security</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Makeup Artist</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Governance</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Cyber Security</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Coding</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Ryan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mcleod</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mendez</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Deacon</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Walker</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Innis</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>West</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Kartel</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Gordon</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>White</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rose Marie</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Moyjah</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Safia</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Sabrina</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Sadiki</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Ricardo</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Kimberly</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Vybes</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Nyikero</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Jonathan</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C66-4324-AA5D-2C38075A5A59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1860538848"/>
+        <c:axId val="1734048496"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Rate</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="10"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Food &amp; Beverage</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Early Childhood</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Makeup Artist</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Governance</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Ryan</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Mcleod</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Mendez</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Deacon</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Walker</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Innis</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>West</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Kartel</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Gordon</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>White</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Rose Marie</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Moyjah</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Safia</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Sabrina</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Sadiki</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Ricardo</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Kimberly</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Vybes</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nyikero</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Jonathan</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$5:$E$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>"$"#,##0.00</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-0C66-4324-AA5D-2C38075A5A59}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Gross Salary</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="10"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Food &amp; Beverage</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Early Childhood</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Makeup Artist</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Governance</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Ryan</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Mcleod</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Mendez</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Deacon</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Walker</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Innis</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>West</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Kartel</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Gordon</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>White</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Rose Marie</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Moyjah</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Safia</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Sabrina</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Sadiki</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Ricardo</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Kimberly</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Vybes</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nyikero</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Jonathan</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$5:$F$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>"$"#,##0.00</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>180000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>157500</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>130000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>167500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>200000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>190000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>222500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>215000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>80000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-0C66-4324-AA5D-2C38075A5A59}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>tax</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="10"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Food &amp; Beverage</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Early Childhood</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Makeup Artist</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Governance</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Ryan</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Mcleod</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Mendez</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Deacon</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Walker</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Innis</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>West</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Kartel</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Gordon</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>White</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Rose Marie</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Moyjah</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Safia</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Sabrina</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Sadiki</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Ricardo</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Kimberly</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Vybes</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nyikero</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Jonathan</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$5:$G$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.32</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.4</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.55000000000000004</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-0C66-4324-AA5D-2C38075A5A59}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Deduction</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="10"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Food &amp; Beverage</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Early Childhood</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Makeup Artist</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Governance</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Ryan</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Mcleod</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Mendez</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Deacon</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Walker</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Innis</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>West</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Kartel</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Gordon</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>White</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Rose Marie</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Moyjah</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Safia</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Sabrina</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Sadiki</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Ricardo</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Kimberly</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Vybes</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nyikero</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Jonathan</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$5:$H$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>"$"#,##0.00</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>15000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>23625</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>41600</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>25125</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>30000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>47500</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>89000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>32250</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>44000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-0C66-4324-AA5D-2C38075A5A59}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Net Pay</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$5:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="10"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Food &amp; Beverage</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Early Childhood</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Makeup Artist</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Governance</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Cyber Security</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Coding</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Ryan</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Mcleod</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Mendez</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Deacon</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Walker</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Innis</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>West</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Kartel</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Gordon</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>White</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Rose Marie</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Moyjah</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Safia</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Sabrina</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Sadiki</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Ricardo</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Kimberly</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Vybes</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nyikero</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Jonathan</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$5:$I$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>"$"#,##0.00</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>85000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>144000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>133875</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>88400</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>142375</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>170000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>142500</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>133500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>182750</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-0C66-4324-AA5D-2C38075A5A59}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1860538848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1734048496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1734048496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1860538848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA02247-606E-44EA-8351-F7FA63E136DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,7 +2520,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +2604,7 @@
       <c r="D5">
         <v>40</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>2500</v>
       </c>
       <c r="F5" s="2">
@@ -631,7 +2614,7 @@
       <c r="G5" s="1">
         <v>0.15</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>(F5*G5)</f>
         <v>15000</v>
       </c>
@@ -653,23 +2636,23 @@
       <c r="D6">
         <v>72</v>
       </c>
-      <c r="E6">
-        <v>5000</v>
+      <c r="E6" s="2">
+        <v>2500</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ref="F6:F14" si="0">PRODUCT(D6:E6)</f>
-        <v>360000</v>
+        <v>180000</v>
       </c>
       <c r="G6" s="1">
         <v>0.2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <f t="shared" ref="H6:H14" si="1">(F6*G6)</f>
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ref="I6:I14" si="2">F6-H6</f>
-        <v>288000</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -685,23 +2668,23 @@
       <c r="D7">
         <v>63</v>
       </c>
-      <c r="E7">
-        <v>5000</v>
+      <c r="E7" s="2">
+        <v>2500</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>315000</v>
+        <v>157500</v>
       </c>
       <c r="G7" s="1">
         <v>0.15</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>47250</v>
+        <v>23625</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="2"/>
-        <v>267750</v>
+        <v>133875</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,23 +2700,23 @@
       <c r="D8">
         <v>52</v>
       </c>
-      <c r="E8">
-        <v>5000</v>
+      <c r="E8" s="2">
+        <v>2500</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>260000</v>
+        <v>130000</v>
       </c>
       <c r="G8" s="1">
         <v>0.32</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>83200</v>
+        <v>41600</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>176800</v>
+        <v>88400</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -749,23 +2732,23 @@
       <c r="D9">
         <v>67</v>
       </c>
-      <c r="E9">
-        <v>6500</v>
+      <c r="E9" s="2">
+        <v>2500</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>435500</v>
+        <v>167500</v>
       </c>
       <c r="G9" s="1">
         <v>0.15</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>65325</v>
+        <v>25125</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="2"/>
-        <v>370175</v>
+        <v>142375</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -781,23 +2764,23 @@
       <c r="D10">
         <v>80</v>
       </c>
-      <c r="E10">
-        <v>4500</v>
+      <c r="E10" s="2">
+        <v>2500</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>360000</v>
+        <v>200000</v>
       </c>
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>54000</v>
+        <v>30000</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="2"/>
-        <v>306000</v>
+        <v>170000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -813,23 +2796,23 @@
       <c r="D11">
         <v>76</v>
       </c>
-      <c r="E11">
-        <v>1200</v>
+      <c r="E11" s="2">
+        <v>2500</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>91200</v>
+        <v>190000</v>
       </c>
       <c r="G11" s="1">
         <v>0.25</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>22800</v>
+        <v>47500</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="2"/>
-        <v>68400</v>
+        <v>142500</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -845,23 +2828,23 @@
       <c r="D12">
         <v>89</v>
       </c>
-      <c r="E12">
-        <v>3200</v>
+      <c r="E12" s="2">
+        <v>2500</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>284800</v>
+        <v>222500</v>
       </c>
       <c r="G12" s="1">
         <v>0.4</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>113920</v>
+        <v>89000</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="2"/>
-        <v>170880</v>
+        <v>133500</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -877,23 +2860,23 @@
       <c r="D13">
         <v>86</v>
       </c>
-      <c r="E13">
-        <v>4000</v>
+      <c r="E13" s="2">
+        <v>2500</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>344000</v>
+        <v>215000</v>
       </c>
       <c r="G13" s="1">
         <v>0.15</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>51600</v>
+        <v>32250</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>292400</v>
+        <v>182750</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -909,23 +2892,23 @@
       <c r="D14">
         <v>32</v>
       </c>
-      <c r="E14">
-        <v>2600</v>
+      <c r="E14" s="2">
+        <v>2500</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>83200</v>
+        <v>80000</v>
       </c>
       <c r="G14" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>45760.000000000007</v>
+        <v>44000</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>37439.999999999993</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,8 +2918,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
=sum(e5:e14) and corrected values in column e(rate)
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B11698-44E9-4D08-B538-6A30F500C437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BC59E-A1E7-46B3-A0AA-B6B05C4264A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -617,31 +617,31 @@
                         <c:v>2500</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2500</c:v>
+                        <c:v>5000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>2500</c:v>
+                        <c:v>5000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2500</c:v>
+                        <c:v>5000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2500</c:v>
+                        <c:v>6500</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2500</c:v>
+                        <c:v>4500</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2500</c:v>
+                        <c:v>1200</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2500</c:v>
+                        <c:v>3200</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2500</c:v>
+                        <c:v>4000</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2500</c:v>
+                        <c:v>2600</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -810,31 +810,31 @@
                         <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>180000</c:v>
+                        <c:v>360000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>157500</c:v>
+                        <c:v>315000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>130000</c:v>
+                        <c:v>260000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>167500</c:v>
+                        <c:v>435500</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>200000</c:v>
+                        <c:v>360000</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>190000</c:v>
+                        <c:v>91200</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>222500</c:v>
+                        <c:v>284800</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>215000</c:v>
+                        <c:v>344000</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>80000</c:v>
+                        <c:v>83200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1196,31 +1196,31 @@
                         <c:v>15000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>36000</c:v>
+                        <c:v>72000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>23625</c:v>
+                        <c:v>47250</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>41600</c:v>
+                        <c:v>83200</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>25125</c:v>
+                        <c:v>65325</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>30000</c:v>
+                        <c:v>54000</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>47500</c:v>
+                        <c:v>22800</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>89000</c:v>
+                        <c:v>113920</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>32250</c:v>
+                        <c:v>51600</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>44000</c:v>
+                        <c:v>45760.000000000007</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1389,31 +1389,31 @@
                         <c:v>85000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>144000</c:v>
+                        <c:v>288000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>133875</c:v>
+                        <c:v>267750</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>88400</c:v>
+                        <c:v>176800</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>142375</c:v>
+                        <c:v>370175</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>170000</c:v>
+                        <c:v>306000</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>142500</c:v>
+                        <c:v>68400</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>133500</c:v>
+                        <c:v>170880</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>182750</c:v>
+                        <c:v>292400</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>36000</c:v>
+                        <c:v>37439.999999999993</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2520,7 +2520,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,22 +2637,22 @@
         <v>72</v>
       </c>
       <c r="E6" s="2">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ref="F6:F14" si="0">PRODUCT(D6:E6)</f>
-        <v>180000</v>
+        <v>360000</v>
       </c>
       <c r="G6" s="1">
         <v>0.2</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ref="H6:H14" si="1">(F6*G6)</f>
-        <v>36000</v>
+        <v>72000</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ref="I6:I14" si="2">F6-H6</f>
-        <v>144000</v>
+        <v>288000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2669,22 +2669,22 @@
         <v>63</v>
       </c>
       <c r="E7" s="2">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>157500</v>
+        <v>315000</v>
       </c>
       <c r="G7" s="1">
         <v>0.15</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>23625</v>
+        <v>47250</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="2"/>
-        <v>133875</v>
+        <v>267750</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2701,22 +2701,22 @@
         <v>52</v>
       </c>
       <c r="E8" s="2">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>130000</v>
+        <v>260000</v>
       </c>
       <c r="G8" s="1">
         <v>0.32</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>41600</v>
+        <v>83200</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>88400</v>
+        <v>176800</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2733,22 +2733,22 @@
         <v>67</v>
       </c>
       <c r="E9" s="2">
-        <v>2500</v>
+        <v>6500</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>167500</v>
+        <v>435500</v>
       </c>
       <c r="G9" s="1">
         <v>0.15</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>25125</v>
+        <v>65325</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="2"/>
-        <v>142375</v>
+        <v>370175</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2765,22 +2765,22 @@
         <v>80</v>
       </c>
       <c r="E10" s="2">
-        <v>2500</v>
+        <v>4500</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>200000</v>
+        <v>360000</v>
       </c>
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>54000</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="2"/>
-        <v>170000</v>
+        <v>306000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2797,22 +2797,22 @@
         <v>76</v>
       </c>
       <c r="E11" s="2">
-        <v>2500</v>
+        <v>1200</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>190000</v>
+        <v>91200</v>
       </c>
       <c r="G11" s="1">
         <v>0.25</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>47500</v>
+        <v>22800</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="2"/>
-        <v>142500</v>
+        <v>68400</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2829,22 +2829,22 @@
         <v>89</v>
       </c>
       <c r="E12" s="2">
-        <v>2500</v>
+        <v>3200</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>222500</v>
+        <v>284800</v>
       </c>
       <c r="G12" s="1">
         <v>0.4</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>89000</v>
+        <v>113920</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="2"/>
-        <v>133500</v>
+        <v>170880</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,22 +2861,22 @@
         <v>86</v>
       </c>
       <c r="E13" s="2">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>215000</v>
+        <v>344000</v>
       </c>
       <c r="G13" s="1">
         <v>0.15</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>32250</v>
+        <v>51600</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>182750</v>
+        <v>292400</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2893,27 +2893,31 @@
         <v>32</v>
       </c>
       <c r="E14" s="2">
-        <v>2500</v>
+        <v>2600</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>80000</v>
+        <v>83200</v>
       </c>
       <c r="G14" s="1">
         <v>0.55000000000000004</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>44000</v>
+        <v>45760.000000000007</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>36000</v>
+        <v>37439.999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
+      </c>
+      <c r="E15" s="2">
+        <f>SUM(E5:E14)</f>
+        <v>39500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
typed =sum(f5:f14) in cell f15 then formated the cell to "number" because i saw "###########"
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BC59E-A1E7-46B3-A0AA-B6B05C4264A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E734C3D2-D4A0-4F9C-B160-64B36CBBDC3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -201,9 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2520,7 +2521,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,21 +2605,21 @@
       <c r="D5">
         <v>40</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>2500</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <f>PRODUCT(D5:E5)</f>
         <v>100000</v>
       </c>
       <c r="G5" s="1">
         <v>0.15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f>(F5*G5)</f>
         <v>15000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <f>F5-H5</f>
         <v>85000</v>
       </c>
@@ -2636,21 +2637,21 @@
       <c r="D6">
         <v>72</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>5000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f t="shared" ref="F6:F14" si="0">PRODUCT(D6:E6)</f>
         <v>360000</v>
       </c>
       <c r="G6" s="1">
         <v>0.2</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f t="shared" ref="H6:H14" si="1">(F6*G6)</f>
         <v>72000</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <f t="shared" ref="I6:I14" si="2">F6-H6</f>
         <v>288000</v>
       </c>
@@ -2668,21 +2669,21 @@
       <c r="D7">
         <v>63</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>5000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>315000</v>
       </c>
       <c r="G7" s="1">
         <v>0.15</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>47250</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <f t="shared" si="2"/>
         <v>267750</v>
       </c>
@@ -2700,21 +2701,21 @@
       <c r="D8">
         <v>52</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>5000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>260000</v>
       </c>
       <c r="G8" s="1">
         <v>0.32</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>83200</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <f t="shared" si="2"/>
         <v>176800</v>
       </c>
@@ -2732,21 +2733,21 @@
       <c r="D9">
         <v>67</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>6500</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>435500</v>
       </c>
       <c r="G9" s="1">
         <v>0.15</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>65325</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <f t="shared" si="2"/>
         <v>370175</v>
       </c>
@@ -2764,21 +2765,21 @@
       <c r="D10">
         <v>80</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>4500</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>360000</v>
       </c>
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>54000</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <f t="shared" si="2"/>
         <v>306000</v>
       </c>
@@ -2796,21 +2797,21 @@
       <c r="D11">
         <v>76</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>1200</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>91200</v>
       </c>
       <c r="G11" s="1">
         <v>0.25</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>22800</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <f t="shared" si="2"/>
         <v>68400</v>
       </c>
@@ -2828,21 +2829,21 @@
       <c r="D12">
         <v>89</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>3200</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>284800</v>
       </c>
       <c r="G12" s="1">
         <v>0.4</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>113920</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <f t="shared" si="2"/>
         <v>170880</v>
       </c>
@@ -2860,21 +2861,21 @@
       <c r="D13">
         <v>86</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>4000</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>344000</v>
       </c>
       <c r="G13" s="1">
         <v>0.15</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <f t="shared" si="1"/>
         <v>51600</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <f t="shared" si="2"/>
         <v>292400</v>
       </c>
@@ -2892,21 +2893,21 @@
       <c r="D14">
         <v>32</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>2600</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>83200</v>
       </c>
       <c r="G14" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <f t="shared" si="1"/>
         <v>45760.000000000007</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
         <f t="shared" si="2"/>
         <v>37439.999999999993</v>
       </c>
@@ -2915,9 +2916,13 @@
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <f>SUM(E5:E14)</f>
         <v>39500</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(F5:F14)</f>
+        <v>2633700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
typed =sum(h5:h14) in cell h15
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E734C3D2-D4A0-4F9C-B160-64B36CBBDC3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C97B8DC-FD78-4CD4-B0FC-147E40EAF3DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -2521,7 +2521,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,6 +2924,10 @@
         <f>SUM(F5:F14)</f>
         <v>2633700</v>
       </c>
+      <c r="H15" s="3">
+        <f>SUM(H5:H14)</f>
+        <v>570855</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
typed =sum(i5:i14) in cell i15
</commit_message>
<xml_diff>
--- a/Excel_Activity_1-Antonio Fuller.xlsx
+++ b/Excel_Activity_1-Antonio Fuller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeartCoding\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C97B8DC-FD78-4CD4-B0FC-147E40EAF3DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF70E7A0-A688-4412-ACC2-609A8575F114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F94E5CF4-A23B-41B0-A3DF-8316C683603D}"/>
   </bookViews>
@@ -2521,7 +2521,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,6 +2928,10 @@
         <f>SUM(H5:H14)</f>
         <v>570855</v>
       </c>
+      <c r="I15" s="2">
+        <f>SUM(I5:I14)</f>
+        <v>2062845</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>